<commit_message>
Prescales: update PbPb menu prescales for name changes
</commit_message>
<xml_diff>
--- a/Prescales/L1Menu_CollisionsHeavyIons2023_v0_0_5_0.xlsx
+++ b/Prescales/L1Menu_CollisionsHeavyIons2023_v0_0_5_0.xlsx
@@ -6109,14 +6109,14 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>L1_MuShower_OneTight</t>
+          <t>L1_SingleMuShower_Tight</t>
         </is>
       </c>
       <c r="C299" t="n">
         <v>0</v>
       </c>
       <c r="D299" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E299" t="n">
         <v>1</v>
@@ -6128,14 +6128,14 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>L1_MuShower_OneNominal</t>
+          <t>L1_SingleMuShower_Nominal</t>
         </is>
       </c>
       <c r="C300" t="n">
         <v>0</v>
       </c>
       <c r="D300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E300" t="n">
         <v>1</v>
@@ -6147,7 +6147,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>L1_MuShower_OneTight_BptxAND</t>
+          <t>L1_SingleMuShower_Tight_BptxAND</t>
         </is>
       </c>
       <c r="C301" t="n">
@@ -6166,7 +6166,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>L1_MuShower_OneNominal_BptxAND</t>
+          <t>L1_SingleMuShower_Nominal_BptxAND</t>
         </is>
       </c>
       <c r="C302" t="n">
@@ -6812,7 +6812,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>L1_ZDC0_AND</t>
+          <t>L1_ZDC1_AND</t>
         </is>
       </c>
       <c r="C336" t="n">
@@ -6869,7 +6869,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>L1_ZDC0_OR</t>
+          <t>L1_ZDC1_OR</t>
         </is>
       </c>
       <c r="C339" t="n">

</xml_diff>